<commit_message>
Updated with Field Name with standard name and Minor release
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_0.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_0.xlsx
@@ -1,7 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="API-Testing" sheetId="1" r:id="rId4"/>
   </sheets>
@@ -81,34 +84,62 @@
   <si>
     <t>POST</t>
   </si>
+  <si>
+    <t>RequestHeaders</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>ExcludeFields</t>
+  </si>
+  <si>
+    <t>StatusCode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
     </font>
     <font>
-      <color theme="1"/>
       <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
     </font>
     <font>
+      <name val="Consolas"/>
       <b/>
       <color rgb="FF008000"/>
-      <name val="Consolas"/>
+      <sz val="12"/>
     </font>
     <font>
+      <name val="Inconsolata"/>
       <b/>
-      <u/>
-      <sz val="11.0"/>
       <color rgb="FF1155CC"/>
-      <name val="Inconsolata"/>
+      <sz val="11"/>
+      <u val="single"/>
     </font>
-    <font/>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -128,27 +159,17 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -364,19 +385,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="176.14"/>
-    <col customWidth="1" min="6" max="6" width="21.71"/>
-    <col customWidth="1" min="8" max="8" width="23.29"/>
+    <col min="2" max="2" width="18.14" customWidth="1"/>
+    <col min="3" max="3" width="176.14" customWidth="1"/>
+    <col min="6" max="6" width="21.71" customWidth="1"/>
+    <col min="8" max="8" width="23.29" customWidth="1"/>
+    <col min="10" max="10" width="18.42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -396,7 +420,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -405,13 +429,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -434,7 +458,7 @@
         <v>16</v>
       </c>
       <c r="K2" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -460,7 +484,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -470,8 +494,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>